<commit_message>
Added real Cave measurements to sample csv
Added real Cave measurements to sample csv
</commit_message>
<xml_diff>
--- a/src/Sample Data/Sample StalBIAS.xlsx
+++ b/src/Sample Data/Sample StalBIAS.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sample StalBIAS" sheetId="1" r:id="rId1"/>
+    <sheet name="More Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Timestamp</t>
   </si>
@@ -67,12 +67,65 @@
   <si>
     <t>Error cCa app</t>
   </si>
+  <si>
+    <t>Site PR-LA-1 (SW1)</t>
+  </si>
+  <si>
+    <t>SW 1</t>
+  </si>
+  <si>
+    <t>Evaporation</t>
+  </si>
+  <si>
+    <t>SW-1</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>pCO2 (ppm)</t>
+  </si>
+  <si>
+    <r>
+      <t>Temp (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>⁰C)</t>
+    </r>
+  </si>
+  <si>
+    <t>Pressure (hPa)</t>
+  </si>
+  <si>
+    <t>RH (%)</t>
+  </si>
+  <si>
+    <t>Start 50 ml</t>
+  </si>
+  <si>
+    <t>Drips/min</t>
+  </si>
+  <si>
+    <t>Distance to Entrance (m)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,8 +261,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,8 +454,32 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -505,6 +594,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -550,9 +756,80 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="36" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="36" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="19" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="19" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -978,7 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
@@ -1939,4 +2216,814 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="13">
+        <v>414.62</v>
+      </c>
+      <c r="D3" s="14">
+        <v>414.62</v>
+      </c>
+      <c r="E3" s="15">
+        <v>414.62</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13">
+        <v>414.62</v>
+      </c>
+      <c r="H3" s="16">
+        <v>414.62</v>
+      </c>
+      <c r="I3" s="13">
+        <v>414.62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>41337</v>
+      </c>
+      <c r="B4" s="18">
+        <v>41337</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="2">
+        <v>589</v>
+      </c>
+      <c r="E4" s="3">
+        <v>22.4</v>
+      </c>
+      <c r="G4" s="4">
+        <v>99.9</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <f>60/I4</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>41366</v>
+      </c>
+      <c r="B5" s="18">
+        <v>41366</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D5" s="2">
+        <v>688</v>
+      </c>
+      <c r="E5" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="G5" s="4">
+        <v>99.9</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6">
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <f>60/I5</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>41392</v>
+      </c>
+      <c r="B6" s="18">
+        <v>41392</v>
+      </c>
+      <c r="C6" s="21">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D6" s="2">
+        <v>734</v>
+      </c>
+      <c r="E6" s="3">
+        <v>22.7</v>
+      </c>
+      <c r="G6" s="4">
+        <v>99.9</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6">
+        <v>13</v>
+      </c>
+      <c r="J6">
+        <f>60/I6</f>
+        <v>4.615384615384615</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>41424</v>
+      </c>
+      <c r="B7" s="22">
+        <v>41424</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D7" s="24">
+        <v>1259</v>
+      </c>
+      <c r="E7" s="25">
+        <v>22.6</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27">
+        <v>99.9</v>
+      </c>
+      <c r="H7" s="28"/>
+      <c r="I7" s="29">
+        <v>27</v>
+      </c>
+      <c r="J7">
+        <f>60/I7</f>
+        <v>2.2222222222222223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>41458</v>
+      </c>
+      <c r="B8" s="22">
+        <v>41458</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.56527777777777777</v>
+      </c>
+      <c r="D8" s="24">
+        <v>1664</v>
+      </c>
+      <c r="E8" s="25">
+        <v>22.6</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27">
+        <v>99.9</v>
+      </c>
+      <c r="H8" s="28">
+        <v>50</v>
+      </c>
+      <c r="I8" s="29">
+        <v>13</v>
+      </c>
+      <c r="J8">
+        <f>60/I8</f>
+        <v>4.615384615384615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>41474</v>
+      </c>
+      <c r="B9" s="30">
+        <v>41474</v>
+      </c>
+      <c r="C9" s="31">
+        <v>0.56527777777777777</v>
+      </c>
+      <c r="D9" s="24">
+        <v>1581</v>
+      </c>
+      <c r="E9" s="25">
+        <v>22.5</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32">
+        <v>99.9</v>
+      </c>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <f>60/I9</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>41504</v>
+      </c>
+      <c r="B10" s="22">
+        <v>41504</v>
+      </c>
+      <c r="C10" s="23">
+        <v>0.6743055555555556</v>
+      </c>
+      <c r="D10" s="24">
+        <v>1880</v>
+      </c>
+      <c r="E10" s="25">
+        <v>22.6</v>
+      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="26">
+        <v>99.9</v>
+      </c>
+      <c r="H10" s="28">
+        <v>50</v>
+      </c>
+      <c r="I10" s="29">
+        <v>17</v>
+      </c>
+      <c r="J10">
+        <f>60/I10</f>
+        <v>3.5294117647058822</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>41519</v>
+      </c>
+      <c r="B11" s="22">
+        <v>41519</v>
+      </c>
+      <c r="C11" s="23">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="D11" s="24">
+        <v>1753</v>
+      </c>
+      <c r="E11" s="25">
+        <v>22.6</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27">
+        <v>99.9</v>
+      </c>
+      <c r="H11" s="28">
+        <v>50</v>
+      </c>
+      <c r="I11" s="29">
+        <v>18</v>
+      </c>
+      <c r="J11">
+        <f>60/I11</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>41547</v>
+      </c>
+      <c r="B12" s="22">
+        <v>41547</v>
+      </c>
+      <c r="C12" s="23">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="D12" s="24">
+        <v>1120</v>
+      </c>
+      <c r="E12" s="25">
+        <v>22.4</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27">
+        <v>97.2</v>
+      </c>
+      <c r="H12" s="28">
+        <v>50</v>
+      </c>
+      <c r="I12" s="29">
+        <v>22</v>
+      </c>
+      <c r="J12">
+        <f>60/I11</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="33">
+        <v>41582</v>
+      </c>
+      <c r="C13" s="34">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="D13" s="35">
+        <v>960</v>
+      </c>
+      <c r="E13" s="36">
+        <v>22.9</v>
+      </c>
+      <c r="F13" s="37">
+        <v>972.5</v>
+      </c>
+      <c r="G13" s="37">
+        <v>92.7</v>
+      </c>
+      <c r="H13" s="38">
+        <v>50</v>
+      </c>
+      <c r="I13" s="39">
+        <v>17</v>
+      </c>
+      <c r="J13">
+        <f>60/I12</f>
+        <v>2.7272727272727271</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>41607</v>
+      </c>
+      <c r="B14" s="33">
+        <v>41607</v>
+      </c>
+      <c r="C14" s="34">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D14" s="35">
+        <v>830</v>
+      </c>
+      <c r="E14" s="36">
+        <v>22.7</v>
+      </c>
+      <c r="F14" s="37">
+        <v>978.1</v>
+      </c>
+      <c r="G14" s="37">
+        <v>94.4</v>
+      </c>
+      <c r="H14" s="38">
+        <v>50</v>
+      </c>
+      <c r="I14" s="39">
+        <v>19</v>
+      </c>
+      <c r="J14">
+        <f>60/I13</f>
+        <v>3.5294117647058822</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>41645</v>
+      </c>
+      <c r="B15" s="33">
+        <v>41645</v>
+      </c>
+      <c r="C15" s="34">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="D15" s="35">
+        <v>620</v>
+      </c>
+      <c r="E15" s="36">
+        <v>22.4</v>
+      </c>
+      <c r="F15" s="37">
+        <v>977.4</v>
+      </c>
+      <c r="G15" s="37">
+        <v>96.5</v>
+      </c>
+      <c r="H15" s="38">
+        <v>50</v>
+      </c>
+      <c r="I15" s="39">
+        <v>19</v>
+      </c>
+      <c r="J15">
+        <f>60/I14</f>
+        <v>3.1578947368421053</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
+        <v>41679</v>
+      </c>
+      <c r="B16" s="22">
+        <v>41679</v>
+      </c>
+      <c r="C16" s="23">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="D16" s="24">
+        <v>550</v>
+      </c>
+      <c r="E16" s="25">
+        <v>22.4</v>
+      </c>
+      <c r="F16" s="27">
+        <v>979.1</v>
+      </c>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28">
+        <v>50</v>
+      </c>
+      <c r="I16" s="29">
+        <v>17</v>
+      </c>
+      <c r="J16">
+        <f>60/I15</f>
+        <v>3.1578947368421053</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="46"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>41737</v>
+      </c>
+      <c r="B18" s="22">
+        <v>41737</v>
+      </c>
+      <c r="C18" s="23">
+        <v>0.5493055555555556</v>
+      </c>
+      <c r="D18" s="24">
+        <v>630</v>
+      </c>
+      <c r="E18" s="25">
+        <v>22.3</v>
+      </c>
+      <c r="F18" s="27">
+        <v>979.1</v>
+      </c>
+      <c r="G18" s="27">
+        <v>99.9</v>
+      </c>
+      <c r="H18" s="28">
+        <v>50</v>
+      </c>
+      <c r="I18" s="29">
+        <v>17</v>
+      </c>
+      <c r="J18">
+        <f>60/I16</f>
+        <v>3.5294117647058822</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="22">
+        <v>41759</v>
+      </c>
+      <c r="C19" s="23">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="D19" s="24">
+        <v>680</v>
+      </c>
+      <c r="E19" s="25">
+        <v>22.4</v>
+      </c>
+      <c r="F19" s="27">
+        <v>978.5</v>
+      </c>
+      <c r="G19" s="27">
+        <v>99.5</v>
+      </c>
+      <c r="H19" s="28">
+        <v>50</v>
+      </c>
+      <c r="I19" s="29">
+        <v>15</v>
+      </c>
+      <c r="J19">
+        <f>60/I18</f>
+        <v>3.5294117647058822</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="22">
+        <v>41790</v>
+      </c>
+      <c r="C20" s="23">
+        <v>0.59513888888888888</v>
+      </c>
+      <c r="D20" s="24">
+        <v>980</v>
+      </c>
+      <c r="E20" s="25">
+        <v>22.2</v>
+      </c>
+      <c r="F20" s="47">
+        <v>976.8</v>
+      </c>
+      <c r="G20" s="48">
+        <v>102.4</v>
+      </c>
+      <c r="H20" s="28">
+        <v>50</v>
+      </c>
+      <c r="I20" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="22">
+        <v>41823</v>
+      </c>
+      <c r="C21" s="23">
+        <v>0.5625</v>
+      </c>
+      <c r="D21" s="24">
+        <v>1420</v>
+      </c>
+      <c r="E21" s="25">
+        <v>22.5</v>
+      </c>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27">
+        <v>102.9</v>
+      </c>
+      <c r="H21" s="28">
+        <v>50</v>
+      </c>
+      <c r="I21" s="29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="22">
+        <v>41852</v>
+      </c>
+      <c r="C22" s="23">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="D22" s="24">
+        <v>1400</v>
+      </c>
+      <c r="E22" s="25">
+        <v>22.3</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27">
+        <v>104.7</v>
+      </c>
+      <c r="H22" s="28">
+        <v>50</v>
+      </c>
+      <c r="I22" s="29"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="49">
+        <v>41883</v>
+      </c>
+      <c r="C23" s="50">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D23" s="14">
+        <v>1750</v>
+      </c>
+      <c r="E23" s="15">
+        <v>22.6</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13">
+        <v>101.56</v>
+      </c>
+      <c r="H23" s="16">
+        <v>50</v>
+      </c>
+      <c r="I23" s="51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="49">
+        <v>41886</v>
+      </c>
+      <c r="C24" s="50">
+        <v>0.51874999999999993</v>
+      </c>
+      <c r="D24" s="14">
+        <v>1880</v>
+      </c>
+      <c r="E24" s="15">
+        <v>23</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="52">
+        <v>100.3</v>
+      </c>
+      <c r="H24" s="16">
+        <v>50</v>
+      </c>
+      <c r="I24" s="51"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="18">
+        <v>41916</v>
+      </c>
+      <c r="C25" s="21">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1010</v>
+      </c>
+      <c r="E25" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="G25" s="12">
+        <v>106.6</v>
+      </c>
+      <c r="H25" s="5">
+        <v>50</v>
+      </c>
+      <c r="I25" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="18">
+        <v>41945</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="22">
+        <v>41978</v>
+      </c>
+      <c r="C27" s="23">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D27" s="24">
+        <v>910</v>
+      </c>
+      <c r="E27" s="25">
+        <v>22.46</v>
+      </c>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27">
+        <v>103.43</v>
+      </c>
+      <c r="H27" s="28">
+        <v>50</v>
+      </c>
+      <c r="I27" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="53">
+        <v>42017</v>
+      </c>
+      <c r="C29" s="54">
+        <v>0.53194444444444444</v>
+      </c>
+      <c r="D29" s="55">
+        <v>760</v>
+      </c>
+      <c r="E29" s="56">
+        <v>22.32</v>
+      </c>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57">
+        <v>104.3</v>
+      </c>
+      <c r="H29" s="58">
+        <v>50</v>
+      </c>
+      <c r="I29" s="59">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="60">
+        <v>42053</v>
+      </c>
+      <c r="C30" s="20">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="D30" s="61">
+        <v>680</v>
+      </c>
+      <c r="E30" s="62">
+        <v>22.3</v>
+      </c>
+      <c r="F30" s="63"/>
+      <c r="G30" s="64">
+        <v>104.39</v>
+      </c>
+      <c r="H30" s="65">
+        <v>50</v>
+      </c>
+      <c r="I30" s="66">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="67">
+        <v>42113</v>
+      </c>
+      <c r="C31" s="68">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D31" s="69">
+        <v>620</v>
+      </c>
+      <c r="E31" s="70">
+        <v>22.5</v>
+      </c>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47">
+        <v>99.92</v>
+      </c>
+      <c r="H31" s="71">
+        <v>50</v>
+      </c>
+      <c r="I31" s="72">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rolf Update Excel Student T test
</commit_message>
<xml_diff>
--- a/src/Sample Data/Sample StalBIAS.xlsx
+++ b/src/Sample Data/Sample StalBIAS.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sample StalBIAS" sheetId="1" r:id="rId1"/>
-    <sheet name="More Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Student T Test-Mattey" sheetId="3" r:id="rId1"/>
+    <sheet name="Sample StalBIAS" sheetId="1" r:id="rId2"/>
+    <sheet name="More Data" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>Timestamp</t>
   </si>
@@ -117,6 +118,108 @@
   <si>
     <t>Distance to Entrance (m)</t>
   </si>
+  <si>
+    <t>FG</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>26/05/05</t>
+  </si>
+  <si>
+    <t>28/04/05</t>
+  </si>
+  <si>
+    <t>23/06/05</t>
+  </si>
+  <si>
+    <t>23/07/05</t>
+  </si>
+  <si>
+    <t>27/0805</t>
+  </si>
+  <si>
+    <t>21/09/05</t>
+  </si>
+  <si>
+    <t>18/10/05</t>
+  </si>
+  <si>
+    <t>30/11/05</t>
+  </si>
+  <si>
+    <t>25/12/05</t>
+  </si>
+  <si>
+    <t>24/05/06</t>
+  </si>
+  <si>
+    <t>25/06/06</t>
+  </si>
+  <si>
+    <t>21/05/06</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>t-Test: Two-Sample Assuming Unequal Variances</t>
+  </si>
+  <si>
+    <t>Variable 1</t>
+  </si>
+  <si>
+    <t>Variable 2</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Hypothesized Mean Difference</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) one-tail</t>
+  </si>
+  <si>
+    <t>t Critical one-tail</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) two-tail</t>
+  </si>
+  <si>
+    <t>t Critical two-tail</t>
+  </si>
+  <si>
+    <t>Var</t>
+  </si>
+  <si>
+    <t>&gt;&gt; We reject null-Hypothesis 10.3 The observed difference between</t>
+  </si>
+  <si>
+    <t>the means is significant with 95%</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Varience</t>
+  </si>
 </sst>
 </file>
 
@@ -125,7 +228,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +372,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -479,7 +590,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -711,6 +822,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -756,7 +887,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -830,6 +961,13 @@
     <xf numFmtId="0" fontId="19" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -886,6 +1024,163 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>467777</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>162524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4152900" y="638175"/>
+          <a:ext cx="7535327" cy="4286849"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>77126</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>585</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8496300" y="5734050"/>
+          <a:ext cx="6630326" cy="4191585"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>771784</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>106</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5715000" y="9734550"/>
+          <a:ext cx="1857634" cy="762106"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>53543</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>781992</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5959043" y="10763251"/>
+          <a:ext cx="1814299" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1253,6 +1548,721 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>2.8850000000000002E-4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>-7.8139999999999994E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>8.4190000000000005E-5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>-1.2109999999999999E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>1.6479999999999999E-4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <v>1.963E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>1.058E-4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>-4.6190000000000003E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="73">
+        <v>38809</v>
+      </c>
+      <c r="B6">
+        <v>1.0179999999999999E-4</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <v>1.6990000000000002E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="74">
+        <v>38782</v>
+      </c>
+      <c r="B7">
+        <v>1.4650000000000001E-4</v>
+      </c>
+      <c r="E7">
+        <v>-8.2639999999999995E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="73">
+        <v>38811</v>
+      </c>
+      <c r="B8">
+        <v>1.784E-4</v>
+      </c>
+      <c r="E8">
+        <v>-5.0599999999999997E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9">
+        <v>1.6349999999999999E-4</v>
+      </c>
+      <c r="E9">
+        <v>-3.1600000000000002E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>1.6349999999999999E-4</v>
+      </c>
+      <c r="E10">
+        <v>-6.2710000000000001E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>1.181E-4</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11">
+        <v>-2.6509999999999999E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1.1129999999999999E-4</v>
+      </c>
+      <c r="E12">
+        <v>1.9700000000000001E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>9.8640000000000004E-5</v>
+      </c>
+      <c r="E13">
+        <f>-0.000020192</f>
+        <v>-2.0191999999999999E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>9.9259999999999995E-5</v>
+      </c>
+      <c r="E14">
+        <v>-1.1610000000000001E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>6.6000000000000005E-5</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15">
+        <v>-3.4709999999999998E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1.026E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2.3450000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18">
+        <v>6.8388999999999999E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>6.7249999999999995E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1.4090000000000001E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1.2410000000000001E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1.415E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25">
+        <f>AVERAGE(B2:B22)</f>
+        <v>1.3188233333333334E-4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25">
+        <f>AVERAGE(E2:E15)</f>
+        <v>-2.8620857142857143E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26">
+        <f>_xlfn.STDEV.P(B2:B22)</f>
+        <v>5.3809047020643671E-5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26">
+        <f>_xlfn.STDEV.P(E2:E15)</f>
+        <v>3.2459725786310164E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27">
+        <f>B26^2</f>
+        <v>2.8954135412698414E-9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27">
+        <f>E26^2</f>
+        <v>1.0536337981224489E-9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28">
+        <f>COUNT(B2:B22)</f>
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28">
+        <f>COUNT(E2:E15)</f>
+        <v>14</v>
+      </c>
+      <c r="I28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29">
+        <f>SUM(B2:B22)</f>
+        <v>2.7695290000000002E-3</v>
+      </c>
+      <c r="E29">
+        <f>SUM(E2:E15)</f>
+        <v>-4.0069200000000002E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="I31" t="s">
+        <v>44</v>
+      </c>
+      <c r="J31">
+        <v>1.3188233333333334E-4</v>
+      </c>
+      <c r="K31">
+        <v>-2.8620857142857143E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I32" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32">
+        <v>3.040184218333334E-9</v>
+      </c>
+      <c r="K32">
+        <v>1.1346825518241757E-9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="77"/>
+      <c r="B33" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33">
+        <f>(B2-$B$25)^2</f>
+        <v>2.4529093512111114E-8</v>
+      </c>
+      <c r="G33">
+        <f>(E2-$E$25)^2</f>
+        <v>2.4521455093061213E-9</v>
+      </c>
+      <c r="I33" t="s">
+        <v>51</v>
+      </c>
+      <c r="J33">
+        <v>21</v>
+      </c>
+      <c r="K33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="75">
+        <v>1.3188233333333334E-4</v>
+      </c>
+      <c r="C34" s="75">
+        <v>-2.8391692307692307E-5</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ref="F34:F53" si="0">(B3-$B$25)^2</f>
+        <v>2.2745586587777781E-9</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ref="G33:G46" si="1">(E3-$E$25)^2</f>
+        <v>2.7260840359183671E-10</v>
+      </c>
+      <c r="I34" t="s">
+        <v>52</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="75" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="75">
+        <v>3.040184218333334E-9</v>
+      </c>
+      <c r="C35" s="75">
+        <v>1.2284429305641026E-9</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>1.0835727787777767E-9</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>2.3281452150204086E-9</v>
+      </c>
+      <c r="I35" t="s">
+        <v>53</v>
+      </c>
+      <c r="J35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="75" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="75">
+        <v>21</v>
+      </c>
+      <c r="C36" s="75">
+        <v>13</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>6.8028811211111174E-10</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>3.0867478073469399E-10</v>
+      </c>
+      <c r="I36" t="s">
+        <v>54</v>
+      </c>
+      <c r="J36">
+        <v>10.680781128466815</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="75">
+        <v>0</v>
+      </c>
+      <c r="C37" s="75"/>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>9.049467787777787E-10</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>2.0803502893061224E-9</v>
+      </c>
+      <c r="I37" t="s">
+        <v>55</v>
+      </c>
+      <c r="J37">
+        <v>1.516712594126494E-12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="75">
+        <v>32</v>
+      </c>
+      <c r="C38" s="75"/>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>2.136761787777778E-10</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>2.9180677950204072E-9</v>
+      </c>
+      <c r="I38" t="s">
+        <v>56</v>
+      </c>
+      <c r="J38">
+        <v>1.6923603090303456</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="75">
+        <v>10.361494246423284</v>
+      </c>
+      <c r="C39" s="75"/>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>2.1638933121111102E-9</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>4.8308272073469372E-10</v>
+      </c>
+      <c r="I39" t="s">
+        <v>57</v>
+      </c>
+      <c r="J39">
+        <v>3.033425188252988E-12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="75">
+        <v>4.7208417387017732E-12</v>
+      </c>
+      <c r="C40" s="75"/>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>9.9967684544444323E-10</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>8.8752921632653217E-12</v>
+      </c>
+      <c r="I40" t="s">
+        <v>58</v>
+      </c>
+      <c r="J40">
+        <v>2.0345152974493397</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="75">
+        <v>1.6938887483837093</v>
+      </c>
+      <c r="C41" s="75"/>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>9.9967684544444323E-10</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>1.1620696607346938E-9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" s="75">
+        <v>9.4416834774035463E-12</v>
+      </c>
+      <c r="C42" s="75"/>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>1.8995271211111144E-10</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>4.4557178775510257E-12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="76" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="76">
+        <v>2.0369333434601011</v>
+      </c>
+      <c r="C43" s="76"/>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>4.2363244544444507E-10</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>2.3349052350204083E-9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>1.1050527254444448E-9</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>7.1045632734693886E-11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="46"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>1.0642166321111121E-9</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>2.8936926073469377E-10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>4.3404818454444451E-9</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>3.7077660734693855E-11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>8.5745504544444498E-10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>1.0530385512111111E-8</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>4.031403377777779E-9</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>4.1773385121111131E-9</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>8.1318312111111105E-11</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>6.0564712111111141E-11</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>9.2499512111110874E-11</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>62</v>
+      </c>
+      <c r="F55">
+        <f>SUM(F33:F54)</f>
+        <v>6.0803684366666678E-8</v>
+      </c>
+      <c r="G55">
+        <f>SUM(G33:G46)</f>
+        <v>1.4750873173714283E-8</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>63</v>
+      </c>
+      <c r="F57">
+        <f>F55/(20)</f>
+        <v>3.040184218333334E-9</v>
+      </c>
+      <c r="G57">
+        <f>G55/13</f>
+        <v>1.1346825518241757E-9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -2218,15 +3228,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
@@ -2321,7 +3337,7 @@
         <v>12</v>
       </c>
       <c r="J4">
-        <f>60/I4</f>
+        <f t="shared" ref="J4:J11" si="0">60/I4</f>
         <v>5</v>
       </c>
     </row>
@@ -2349,7 +3365,7 @@
         <v>15</v>
       </c>
       <c r="J5">
-        <f>60/I5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -2377,7 +3393,7 @@
         <v>13</v>
       </c>
       <c r="J6">
-        <f>60/I6</f>
+        <f t="shared" si="0"/>
         <v>4.615384615384615</v>
       </c>
     </row>
@@ -2406,7 +3422,7 @@
         <v>27</v>
       </c>
       <c r="J7">
-        <f>60/I7</f>
+        <f t="shared" si="0"/>
         <v>2.2222222222222223</v>
       </c>
     </row>
@@ -2437,7 +3453,7 @@
         <v>13</v>
       </c>
       <c r="J8">
-        <f>60/I8</f>
+        <f t="shared" si="0"/>
         <v>4.615384615384615</v>
       </c>
     </row>
@@ -2466,7 +3482,7 @@
         <v>10</v>
       </c>
       <c r="J9">
-        <f>60/I9</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -2497,7 +3513,7 @@
         <v>17</v>
       </c>
       <c r="J10">
-        <f>60/I10</f>
+        <f t="shared" si="0"/>
         <v>3.5294117647058822</v>
       </c>
     </row>
@@ -2528,7 +3544,7 @@
         <v>18</v>
       </c>
       <c r="J11">
-        <f>60/I11</f>
+        <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
     </row>

</xml_diff>